<commit_message>
actualización de archivo fem.py
</commit_message>
<xml_diff>
--- a/element_node_ID.xlsx
+++ b/element_node_ID.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\Finite_element_method\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Repositorios\fem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5566906-83E5-4DC5-9BB6-35B42772F1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F345184F-B5E7-41A6-80B2-4DB4EA0FC216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{09F8E42D-5D46-42B5-AA36-B11748BF3332}"/>
   </bookViews>
@@ -25,13 +25,13 @@
     <t>element</t>
   </si>
   <si>
-    <t xml:space="preserve"> LN1</t>
+    <t>Node_1</t>
   </si>
   <si>
-    <t xml:space="preserve"> LN2</t>
+    <t>Node_2</t>
   </si>
   <si>
-    <t xml:space="preserve"> LN3</t>
+    <t>Node_3</t>
   </si>
 </sst>
 </file>
@@ -515,9 +515,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -893,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD1D249-B26F-4DB2-BDB3-FFED6AB3A539}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,9 +942,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>